<commit_message>
calculate excellent for active worker
</commit_message>
<xml_diff>
--- a/IAS19_part2_results.xlsx
+++ b/IAS19_part2_results.xlsx
@@ -512,12 +512,18 @@
       <c r="B2" t="n">
         <v>0</v>
       </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
-      <c r="F2" t="inlineStr"/>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
@@ -548,12 +554,18 @@
       <c r="B3" t="n">
         <v>0</v>
       </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
-      <c r="F3" t="inlineStr"/>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
       <c r="G3" t="n">
         <v>0</v>
       </c>
@@ -672,12 +684,18 @@
       <c r="B6" t="n">
         <v>0</v>
       </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
-      <c r="F6" t="inlineStr"/>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
       <c r="G6" t="n">
         <v>0</v>
       </c>
@@ -752,12 +770,18 @@
       <c r="B8" t="n">
         <v>0</v>
       </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
-      <c r="F8" t="inlineStr"/>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
       <c r="G8" t="n">
         <v>0</v>
       </c>
@@ -832,12 +856,18 @@
       <c r="B10" t="n">
         <v>0</v>
       </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
-      <c r="F10" t="inlineStr"/>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
       <c r="G10" t="n">
         <v>0</v>
       </c>
@@ -956,12 +986,18 @@
       <c r="B13" t="n">
         <v>0</v>
       </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
       <c r="E13" t="n">
         <v>0</v>
       </c>
-      <c r="F13" t="inlineStr"/>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
       <c r="G13" t="n">
         <v>0</v>
       </c>
@@ -992,12 +1028,18 @@
       <c r="B14" t="n">
         <v>200000</v>
       </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>6338.900000000003</v>
+      </c>
       <c r="E14" t="n">
         <v>0</v>
       </c>
-      <c r="F14" t="inlineStr"/>
+      <c r="F14" t="n">
+        <v>146248.1</v>
+      </c>
       <c r="G14" t="n">
         <v>352587</v>
       </c>
@@ -1204,12 +1246,18 @@
       <c r="B19" t="n">
         <v>200000</v>
       </c>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>5598.7</v>
+      </c>
       <c r="E19" t="n">
         <v>0</v>
       </c>
-      <c r="F19" t="inlineStr"/>
+      <c r="F19" t="n">
+        <v>-205598.7</v>
+      </c>
       <c r="G19" t="n">
         <v>0</v>
       </c>
@@ -1240,12 +1288,18 @@
       <c r="B20" t="n">
         <v>200000</v>
       </c>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>6093.500000000001</v>
+      </c>
       <c r="E20" t="n">
         <v>0</v>
       </c>
-      <c r="F20" t="inlineStr"/>
+      <c r="F20" t="n">
+        <v>-137955.5</v>
+      </c>
       <c r="G20" t="n">
         <v>68138</v>
       </c>
@@ -1320,12 +1374,18 @@
       <c r="B22" t="n">
         <v>0</v>
       </c>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
       <c r="E22" t="n">
         <v>0</v>
       </c>
-      <c r="F22" t="inlineStr"/>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
       <c r="G22" t="n">
         <v>0</v>
       </c>
@@ -1400,12 +1460,18 @@
       <c r="B24" t="n">
         <v>200000</v>
       </c>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>5812.147000000002</v>
+      </c>
       <c r="E24" t="n">
         <v>26000</v>
       </c>
-      <c r="F24" t="inlineStr"/>
+      <c r="F24" t="n">
+        <v>-179812.147</v>
+      </c>
       <c r="G24" t="n">
         <v>0</v>
       </c>
@@ -1436,12 +1502,18 @@
       <c r="B25" t="n">
         <v>200000</v>
       </c>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>7075.100000000007</v>
+      </c>
       <c r="E25" t="n">
         <v>0</v>
       </c>
-      <c r="F25" t="inlineStr"/>
+      <c r="F25" t="n">
+        <v>-207075.1</v>
+      </c>
       <c r="G25" t="n">
         <v>0</v>
       </c>
@@ -1472,12 +1544,18 @@
       <c r="B26" t="n">
         <v>200000</v>
       </c>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
+      <c r="C26" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>6461.600000000003</v>
+      </c>
       <c r="E26" t="n">
         <v>0</v>
       </c>
-      <c r="F26" t="inlineStr"/>
+      <c r="F26" t="n">
+        <v>-206461.6</v>
+      </c>
       <c r="G26" t="n">
         <v>0</v>
       </c>
@@ -1508,12 +1586,18 @@
       <c r="B27" t="n">
         <v>200000</v>
       </c>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>6093.500000000001</v>
+      </c>
       <c r="E27" t="n">
         <v>0</v>
       </c>
-      <c r="F27" t="inlineStr"/>
+      <c r="F27" t="n">
+        <v>55458.5</v>
+      </c>
       <c r="G27" t="n">
         <v>261552</v>
       </c>
@@ -1544,12 +1628,18 @@
       <c r="B28" t="n">
         <v>0</v>
       </c>
-      <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
       <c r="E28" t="n">
         <v>0</v>
       </c>
-      <c r="F28" t="inlineStr"/>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
       <c r="G28" t="n">
         <v>0</v>
       </c>
@@ -1624,12 +1714,18 @@
       <c r="B30" t="n">
         <v>200000</v>
       </c>
-      <c r="C30" t="inlineStr"/>
-      <c r="D30" t="inlineStr"/>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>6707.000000000005</v>
+      </c>
       <c r="E30" t="n">
         <v>0</v>
       </c>
-      <c r="F30" t="inlineStr"/>
+      <c r="F30" t="n">
+        <v>-206707</v>
+      </c>
       <c r="G30" t="n">
         <v>0</v>
       </c>
@@ -1660,12 +1756,18 @@
       <c r="B31" t="n">
         <v>200000</v>
       </c>
-      <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr"/>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>7197.800000000007</v>
+      </c>
       <c r="E31" t="n">
         <v>0</v>
       </c>
-      <c r="F31" t="inlineStr"/>
+      <c r="F31" t="n">
+        <v>-207197.8</v>
+      </c>
       <c r="G31" t="n">
         <v>0</v>
       </c>
@@ -1696,12 +1798,18 @@
       <c r="B32" t="n">
         <v>200000</v>
       </c>
-      <c r="C32" t="inlineStr"/>
-      <c r="D32" t="inlineStr"/>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" t="n">
+        <v>7320.500000000007</v>
+      </c>
       <c r="E32" t="n">
         <v>0</v>
       </c>
-      <c r="F32" t="inlineStr"/>
+      <c r="F32" t="n">
+        <v>-207320.5</v>
+      </c>
       <c r="G32" t="n">
         <v>0</v>
       </c>
@@ -1820,12 +1928,18 @@
       <c r="B35" t="n">
         <v>200000</v>
       </c>
-      <c r="C35" t="inlineStr"/>
-      <c r="D35" t="inlineStr"/>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>7075.100000000007</v>
+      </c>
       <c r="E35" t="n">
         <v>0</v>
       </c>
-      <c r="F35" t="inlineStr"/>
+      <c r="F35" t="n">
+        <v>170539.9</v>
+      </c>
       <c r="G35" t="n">
         <v>377615</v>
       </c>
@@ -1856,12 +1970,18 @@
       <c r="B36" t="n">
         <v>200000</v>
       </c>
-      <c r="C36" t="inlineStr"/>
-      <c r="D36" t="inlineStr"/>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" t="n">
+        <v>7565.900000000009</v>
+      </c>
       <c r="E36" t="n">
         <v>0</v>
       </c>
-      <c r="F36" t="inlineStr"/>
+      <c r="F36" t="n">
+        <v>-207565.9</v>
+      </c>
       <c r="G36" t="n">
         <v>0</v>
       </c>
@@ -1892,12 +2012,18 @@
       <c r="B37" t="n">
         <v>200000</v>
       </c>
-      <c r="C37" t="inlineStr"/>
-      <c r="D37" t="inlineStr"/>
+      <c r="C37" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" t="n">
+        <v>6584.300000000004</v>
+      </c>
       <c r="E37" t="n">
         <v>0</v>
       </c>
-      <c r="F37" t="inlineStr"/>
+      <c r="F37" t="n">
+        <v>-206584.3</v>
+      </c>
       <c r="G37" t="n">
         <v>0</v>
       </c>
@@ -1928,12 +2054,18 @@
       <c r="B38" t="n">
         <v>200000</v>
       </c>
-      <c r="C38" t="inlineStr"/>
-      <c r="D38" t="inlineStr"/>
+      <c r="C38" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>6584.300000000004</v>
+      </c>
       <c r="E38" t="n">
         <v>0</v>
       </c>
-      <c r="F38" t="inlineStr"/>
+      <c r="F38" t="n">
+        <v>13546.7</v>
+      </c>
       <c r="G38" t="n">
         <v>220131</v>
       </c>
@@ -2008,12 +2140,18 @@
       <c r="B40" t="n">
         <v>0</v>
       </c>
-      <c r="C40" t="inlineStr"/>
-      <c r="D40" t="inlineStr"/>
+      <c r="C40" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0</v>
+      </c>
       <c r="E40" t="n">
         <v>0</v>
       </c>
-      <c r="F40" t="inlineStr"/>
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
       <c r="G40" t="n">
         <v>0</v>
       </c>
@@ -2044,12 +2182,18 @@
       <c r="B41" t="n">
         <v>0</v>
       </c>
-      <c r="C41" t="inlineStr"/>
-      <c r="D41" t="inlineStr"/>
+      <c r="C41" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0</v>
+      </c>
       <c r="E41" t="n">
         <v>0</v>
       </c>
-      <c r="F41" t="inlineStr"/>
+      <c r="F41" t="n">
+        <v>0</v>
+      </c>
       <c r="G41" t="n">
         <v>0</v>
       </c>
@@ -2080,12 +2224,18 @@
       <c r="B42" t="n">
         <v>200000</v>
       </c>
-      <c r="C42" t="inlineStr"/>
-      <c r="D42" t="inlineStr"/>
+      <c r="C42" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" t="n">
+        <v>3629.3</v>
+      </c>
       <c r="E42" t="n">
         <v>0</v>
       </c>
-      <c r="F42" t="inlineStr"/>
+      <c r="F42" t="n">
+        <v>-123629.3</v>
+      </c>
       <c r="G42" t="n">
         <v>80000</v>
       </c>
@@ -2116,12 +2266,18 @@
       <c r="B43" t="n">
         <v>0</v>
       </c>
-      <c r="C43" t="inlineStr"/>
-      <c r="D43" t="inlineStr"/>
+      <c r="C43" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0</v>
+      </c>
       <c r="E43" t="n">
         <v>0</v>
       </c>
-      <c r="F43" t="inlineStr"/>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
       <c r="G43" t="n">
         <v>0</v>
       </c>
@@ -2152,12 +2308,18 @@
       <c r="B44" t="n">
         <v>0</v>
       </c>
-      <c r="C44" t="inlineStr"/>
-      <c r="D44" t="inlineStr"/>
+      <c r="C44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
       <c r="E44" t="n">
         <v>0</v>
       </c>
-      <c r="F44" t="inlineStr"/>
+      <c r="F44" t="n">
+        <v>0</v>
+      </c>
       <c r="G44" t="n">
         <v>0</v>
       </c>
@@ -2408,12 +2570,18 @@
       <c r="B50" t="n">
         <v>200000</v>
       </c>
-      <c r="C50" t="inlineStr"/>
-      <c r="D50" t="inlineStr"/>
+      <c r="C50" t="n">
+        <v>0</v>
+      </c>
+      <c r="D50" t="n">
+        <v>2812.7075</v>
+      </c>
       <c r="E50" t="n">
         <v>90000</v>
       </c>
-      <c r="F50" t="inlineStr"/>
+      <c r="F50" t="n">
+        <v>-112812.7075</v>
+      </c>
       <c r="G50" t="n">
         <v>0</v>
       </c>
@@ -2444,12 +2612,18 @@
       <c r="B51" t="n">
         <v>0</v>
       </c>
-      <c r="C51" t="inlineStr"/>
-      <c r="D51" t="inlineStr"/>
+      <c r="C51" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0</v>
+      </c>
       <c r="E51" t="n">
         <v>0</v>
       </c>
-      <c r="F51" t="inlineStr"/>
+      <c r="F51" t="n">
+        <v>0</v>
+      </c>
       <c r="G51" t="n">
         <v>0</v>
       </c>
@@ -2524,12 +2698,18 @@
       <c r="B53" t="n">
         <v>0</v>
       </c>
-      <c r="C53" t="inlineStr"/>
-      <c r="D53" t="inlineStr"/>
+      <c r="C53" t="n">
+        <v>0</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0</v>
+      </c>
       <c r="E53" t="n">
         <v>0</v>
       </c>
-      <c r="F53" t="inlineStr"/>
+      <c r="F53" t="n">
+        <v>0</v>
+      </c>
       <c r="G53" t="n">
         <v>0</v>
       </c>
@@ -2560,12 +2740,18 @@
       <c r="B54" t="n">
         <v>0</v>
       </c>
-      <c r="C54" t="inlineStr"/>
-      <c r="D54" t="inlineStr"/>
+      <c r="C54" t="n">
+        <v>0</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0</v>
+      </c>
       <c r="E54" t="n">
         <v>0</v>
       </c>
-      <c r="F54" t="inlineStr"/>
+      <c r="F54" t="n">
+        <v>0</v>
+      </c>
       <c r="G54" t="n">
         <v>0</v>
       </c>
@@ -2596,12 +2782,18 @@
       <c r="B55" t="n">
         <v>0</v>
       </c>
-      <c r="C55" t="inlineStr"/>
-      <c r="D55" t="inlineStr"/>
+      <c r="C55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0</v>
+      </c>
       <c r="E55" t="n">
         <v>0</v>
       </c>
-      <c r="F55" t="inlineStr"/>
+      <c r="F55" t="n">
+        <v>0</v>
+      </c>
       <c r="G55" t="n">
         <v>0</v>
       </c>
@@ -2632,12 +2824,18 @@
       <c r="B56" t="n">
         <v>0</v>
       </c>
-      <c r="C56" t="inlineStr"/>
-      <c r="D56" t="inlineStr"/>
+      <c r="C56" t="n">
+        <v>0</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0</v>
+      </c>
       <c r="E56" t="n">
         <v>0</v>
       </c>
-      <c r="F56" t="inlineStr"/>
+      <c r="F56" t="n">
+        <v>0</v>
+      </c>
       <c r="G56" t="n">
         <v>0</v>
       </c>
@@ -2712,12 +2910,18 @@
       <c r="B58" t="n">
         <v>0</v>
       </c>
-      <c r="C58" t="inlineStr"/>
-      <c r="D58" t="inlineStr"/>
+      <c r="C58" t="n">
+        <v>0</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0</v>
+      </c>
       <c r="E58" t="n">
         <v>0</v>
       </c>
-      <c r="F58" t="inlineStr"/>
+      <c r="F58" t="n">
+        <v>0</v>
+      </c>
       <c r="G58" t="n">
         <v>0</v>
       </c>
@@ -2748,12 +2952,18 @@
       <c r="B59" t="n">
         <v>0</v>
       </c>
-      <c r="C59" t="inlineStr"/>
-      <c r="D59" t="inlineStr"/>
+      <c r="C59" t="n">
+        <v>0</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0</v>
+      </c>
       <c r="E59" t="n">
         <v>0</v>
       </c>
-      <c r="F59" t="inlineStr"/>
+      <c r="F59" t="n">
+        <v>0</v>
+      </c>
       <c r="G59" t="n">
         <v>0</v>
       </c>
@@ -2784,12 +2994,18 @@
       <c r="B60" t="n">
         <v>0</v>
       </c>
-      <c r="C60" t="inlineStr"/>
-      <c r="D60" t="inlineStr"/>
+      <c r="C60" t="n">
+        <v>0</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0</v>
+      </c>
       <c r="E60" t="n">
         <v>0</v>
       </c>
-      <c r="F60" t="inlineStr"/>
+      <c r="F60" t="n">
+        <v>0</v>
+      </c>
       <c r="G60" t="n">
         <v>0</v>
       </c>
@@ -2908,12 +3124,18 @@
       <c r="B63" t="n">
         <v>0</v>
       </c>
-      <c r="C63" t="inlineStr"/>
-      <c r="D63" t="inlineStr"/>
+      <c r="C63" t="n">
+        <v>0</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0</v>
+      </c>
       <c r="E63" t="n">
         <v>0</v>
       </c>
-      <c r="F63" t="inlineStr"/>
+      <c r="F63" t="n">
+        <v>0</v>
+      </c>
       <c r="G63" t="n">
         <v>0</v>
       </c>
@@ -2944,12 +3166,18 @@
       <c r="B64" t="n">
         <v>0</v>
       </c>
-      <c r="C64" t="inlineStr"/>
-      <c r="D64" t="inlineStr"/>
+      <c r="C64" t="n">
+        <v>0</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0</v>
+      </c>
       <c r="E64" t="n">
         <v>0</v>
       </c>
-      <c r="F64" t="inlineStr"/>
+      <c r="F64" t="n">
+        <v>0</v>
+      </c>
       <c r="G64" t="n">
         <v>0</v>
       </c>
@@ -3068,12 +3296,18 @@
       <c r="B67" t="n">
         <v>0</v>
       </c>
-      <c r="C67" t="inlineStr"/>
-      <c r="D67" t="inlineStr"/>
+      <c r="C67" t="n">
+        <v>0</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0</v>
+      </c>
       <c r="E67" t="n">
         <v>0</v>
       </c>
-      <c r="F67" t="inlineStr"/>
+      <c r="F67" t="n">
+        <v>0</v>
+      </c>
       <c r="G67" t="n">
         <v>0</v>
       </c>
@@ -3236,12 +3470,18 @@
       <c r="B71" t="n">
         <v>200000</v>
       </c>
-      <c r="C71" t="inlineStr"/>
-      <c r="D71" t="inlineStr"/>
+      <c r="C71" t="n">
+        <v>0</v>
+      </c>
+      <c r="D71" t="n">
+        <v>5848.099999999999</v>
+      </c>
       <c r="E71" t="n">
         <v>0</v>
       </c>
-      <c r="F71" t="inlineStr"/>
+      <c r="F71" t="n">
+        <v>-205848.1</v>
+      </c>
       <c r="G71" t="n">
         <v>0</v>
       </c>
@@ -3360,12 +3600,18 @@
       <c r="B74" t="n">
         <v>200000</v>
       </c>
-      <c r="C74" t="inlineStr"/>
-      <c r="D74" t="inlineStr"/>
+      <c r="C74" t="n">
+        <v>0</v>
+      </c>
+      <c r="D74" t="n">
+        <v>5848.099999999999</v>
+      </c>
       <c r="E74" t="n">
         <v>0</v>
       </c>
-      <c r="F74" t="inlineStr"/>
+      <c r="F74" t="n">
+        <v>-43000.1</v>
+      </c>
       <c r="G74" t="n">
         <v>162848</v>
       </c>
@@ -3528,12 +3774,18 @@
       <c r="B78" t="n">
         <v>0</v>
       </c>
-      <c r="C78" t="inlineStr"/>
-      <c r="D78" t="inlineStr"/>
+      <c r="C78" t="n">
+        <v>0</v>
+      </c>
+      <c r="D78" t="n">
+        <v>0</v>
+      </c>
       <c r="E78" t="n">
         <v>0</v>
       </c>
-      <c r="F78" t="inlineStr"/>
+      <c r="F78" t="n">
+        <v>0</v>
+      </c>
       <c r="G78" t="n">
         <v>0</v>
       </c>
@@ -3564,12 +3816,18 @@
       <c r="B79" t="n">
         <v>200000</v>
       </c>
-      <c r="C79" t="inlineStr"/>
-      <c r="D79" t="inlineStr"/>
+      <c r="C79" t="n">
+        <v>0</v>
+      </c>
+      <c r="D79" t="n">
+        <v>5598.7</v>
+      </c>
       <c r="E79" t="n">
         <v>0</v>
       </c>
-      <c r="F79" t="inlineStr"/>
+      <c r="F79" t="n">
+        <v>-205598.7</v>
+      </c>
       <c r="G79" t="n">
         <v>0</v>
       </c>
@@ -3644,12 +3902,18 @@
       <c r="B81" t="n">
         <v>0</v>
       </c>
-      <c r="C81" t="inlineStr"/>
-      <c r="D81" t="inlineStr"/>
+      <c r="C81" t="n">
+        <v>0</v>
+      </c>
+      <c r="D81" t="n">
+        <v>0</v>
+      </c>
       <c r="E81" t="n">
         <v>0</v>
       </c>
-      <c r="F81" t="inlineStr"/>
+      <c r="F81" t="n">
+        <v>0</v>
+      </c>
       <c r="G81" t="n">
         <v>0</v>
       </c>
@@ -3724,12 +3988,18 @@
       <c r="B83" t="n">
         <v>0</v>
       </c>
-      <c r="C83" t="inlineStr"/>
-      <c r="D83" t="inlineStr"/>
+      <c r="C83" t="n">
+        <v>0</v>
+      </c>
+      <c r="D83" t="n">
+        <v>0</v>
+      </c>
       <c r="E83" t="n">
         <v>0</v>
       </c>
-      <c r="F83" t="inlineStr"/>
+      <c r="F83" t="n">
+        <v>0</v>
+      </c>
       <c r="G83" t="n">
         <v>0</v>
       </c>
@@ -3760,12 +4030,18 @@
       <c r="B84" t="n">
         <v>200000</v>
       </c>
-      <c r="C84" t="inlineStr"/>
-      <c r="D84" t="inlineStr"/>
+      <c r="C84" t="n">
+        <v>0</v>
+      </c>
+      <c r="D84" t="n">
+        <v>5761.262500000003</v>
+      </c>
       <c r="E84" t="n">
         <v>50000</v>
       </c>
-      <c r="F84" t="inlineStr"/>
+      <c r="F84" t="n">
+        <v>-155761.2625</v>
+      </c>
       <c r="G84" t="n">
         <v>0</v>
       </c>
@@ -3796,12 +4072,18 @@
       <c r="B85" t="n">
         <v>0</v>
       </c>
-      <c r="C85" t="inlineStr"/>
-      <c r="D85" t="inlineStr"/>
+      <c r="C85" t="n">
+        <v>0</v>
+      </c>
+      <c r="D85" t="n">
+        <v>0</v>
+      </c>
       <c r="E85" t="n">
         <v>0</v>
       </c>
-      <c r="F85" t="inlineStr"/>
+      <c r="F85" t="n">
+        <v>0</v>
+      </c>
       <c r="G85" t="n">
         <v>0</v>
       </c>
@@ -3876,12 +4158,18 @@
       <c r="B87" t="n">
         <v>0</v>
       </c>
-      <c r="C87" t="inlineStr"/>
-      <c r="D87" t="inlineStr"/>
+      <c r="C87" t="n">
+        <v>0</v>
+      </c>
+      <c r="D87" t="n">
+        <v>0</v>
+      </c>
       <c r="E87" t="n">
         <v>0</v>
       </c>
-      <c r="F87" t="inlineStr"/>
+      <c r="F87" t="n">
+        <v>0</v>
+      </c>
       <c r="G87" t="n">
         <v>0</v>
       </c>
@@ -3912,12 +4200,18 @@
       <c r="B88" t="n">
         <v>0</v>
       </c>
-      <c r="C88" t="inlineStr"/>
-      <c r="D88" t="inlineStr"/>
+      <c r="C88" t="n">
+        <v>0</v>
+      </c>
+      <c r="D88" t="n">
+        <v>0</v>
+      </c>
       <c r="E88" t="n">
         <v>0</v>
       </c>
-      <c r="F88" t="inlineStr"/>
+      <c r="F88" t="n">
+        <v>0</v>
+      </c>
       <c r="G88" t="n">
         <v>0</v>
       </c>
@@ -4036,12 +4330,18 @@
       <c r="B91" t="n">
         <v>200000</v>
       </c>
-      <c r="C91" t="inlineStr"/>
-      <c r="D91" t="inlineStr"/>
+      <c r="C91" t="n">
+        <v>0</v>
+      </c>
+      <c r="D91" t="n">
+        <v>7320.500000000007</v>
+      </c>
       <c r="E91" t="n">
         <v>0</v>
       </c>
-      <c r="F91" t="inlineStr"/>
+      <c r="F91" t="n">
+        <v>-175181.5</v>
+      </c>
       <c r="G91" t="n">
         <v>32139</v>
       </c>
@@ -4116,12 +4416,18 @@
       <c r="B93" t="n">
         <v>0</v>
       </c>
-      <c r="C93" t="inlineStr"/>
-      <c r="D93" t="inlineStr"/>
+      <c r="C93" t="n">
+        <v>0</v>
+      </c>
+      <c r="D93" t="n">
+        <v>0</v>
+      </c>
       <c r="E93" t="n">
         <v>0</v>
       </c>
-      <c r="F93" t="inlineStr"/>
+      <c r="F93" t="n">
+        <v>0</v>
+      </c>
       <c r="G93" t="n">
         <v>0</v>
       </c>
@@ -4152,12 +4458,18 @@
       <c r="B94" t="n">
         <v>0</v>
       </c>
-      <c r="C94" t="inlineStr"/>
-      <c r="D94" t="inlineStr"/>
+      <c r="C94" t="n">
+        <v>0</v>
+      </c>
+      <c r="D94" t="n">
+        <v>0</v>
+      </c>
       <c r="E94" t="n">
         <v>0</v>
       </c>
-      <c r="F94" t="inlineStr"/>
+      <c r="F94" t="n">
+        <v>0</v>
+      </c>
       <c r="G94" t="n">
         <v>0</v>
       </c>
@@ -4232,12 +4544,18 @@
       <c r="B96" t="n">
         <v>0</v>
       </c>
-      <c r="C96" t="inlineStr"/>
-      <c r="D96" t="inlineStr"/>
+      <c r="C96" t="n">
+        <v>0</v>
+      </c>
+      <c r="D96" t="n">
+        <v>0</v>
+      </c>
       <c r="E96" t="n">
         <v>0</v>
       </c>
-      <c r="F96" t="inlineStr"/>
+      <c r="F96" t="n">
+        <v>0</v>
+      </c>
       <c r="G96" t="n">
         <v>0</v>
       </c>
@@ -4268,12 +4586,18 @@
       <c r="B97" t="n">
         <v>0</v>
       </c>
-      <c r="C97" t="inlineStr"/>
-      <c r="D97" t="inlineStr"/>
+      <c r="C97" t="n">
+        <v>0</v>
+      </c>
+      <c r="D97" t="n">
+        <v>0</v>
+      </c>
       <c r="E97" t="n">
         <v>0</v>
       </c>
-      <c r="F97" t="inlineStr"/>
+      <c r="F97" t="n">
+        <v>0</v>
+      </c>
       <c r="G97" t="n">
         <v>0</v>
       </c>
@@ -4436,12 +4760,18 @@
       <c r="B101" t="n">
         <v>0</v>
       </c>
-      <c r="C101" t="inlineStr"/>
-      <c r="D101" t="inlineStr"/>
+      <c r="C101" t="n">
+        <v>0</v>
+      </c>
+      <c r="D101" t="n">
+        <v>0</v>
+      </c>
       <c r="E101" t="n">
         <v>0</v>
       </c>
-      <c r="F101" t="inlineStr"/>
+      <c r="F101" t="n">
+        <v>0</v>
+      </c>
       <c r="G101" t="n">
         <v>0</v>
       </c>
@@ -4472,12 +4802,18 @@
       <c r="B102" t="n">
         <v>200000</v>
       </c>
-      <c r="C102" t="inlineStr"/>
-      <c r="D102" t="inlineStr"/>
+      <c r="C102" t="n">
+        <v>0</v>
+      </c>
+      <c r="D102" t="n">
+        <v>7075.100000000007</v>
+      </c>
       <c r="E102" t="n">
         <v>0</v>
       </c>
-      <c r="F102" t="inlineStr"/>
+      <c r="F102" t="n">
+        <v>-128627.1</v>
+      </c>
       <c r="G102" t="n">
         <v>78448</v>
       </c>
@@ -4596,12 +4932,18 @@
       <c r="B105" t="n">
         <v>0</v>
       </c>
-      <c r="C105" t="inlineStr"/>
-      <c r="D105" t="inlineStr"/>
+      <c r="C105" t="n">
+        <v>0</v>
+      </c>
+      <c r="D105" t="n">
+        <v>0</v>
+      </c>
       <c r="E105" t="n">
         <v>0</v>
       </c>
-      <c r="F105" t="inlineStr"/>
+      <c r="F105" t="n">
+        <v>0</v>
+      </c>
       <c r="G105" t="n">
         <v>0</v>
       </c>
@@ -4632,12 +4974,18 @@
       <c r="B106" t="n">
         <v>0</v>
       </c>
-      <c r="C106" t="inlineStr"/>
-      <c r="D106" t="inlineStr"/>
+      <c r="C106" t="n">
+        <v>0</v>
+      </c>
+      <c r="D106" t="n">
+        <v>0</v>
+      </c>
       <c r="E106" t="n">
         <v>0</v>
       </c>
-      <c r="F106" t="inlineStr"/>
+      <c r="F106" t="n">
+        <v>0</v>
+      </c>
       <c r="G106" t="n">
         <v>0</v>
       </c>
@@ -5108,12 +5456,18 @@
       <c r="B117" t="n">
         <v>0</v>
       </c>
-      <c r="C117" t="inlineStr"/>
-      <c r="D117" t="inlineStr"/>
+      <c r="C117" t="n">
+        <v>0</v>
+      </c>
+      <c r="D117" t="n">
+        <v>0</v>
+      </c>
       <c r="E117" t="n">
         <v>0</v>
       </c>
-      <c r="F117" t="inlineStr"/>
+      <c r="F117" t="n">
+        <v>0</v>
+      </c>
       <c r="G117" t="n">
         <v>0</v>
       </c>
@@ -5276,12 +5630,18 @@
       <c r="B121" t="n">
         <v>0</v>
       </c>
-      <c r="C121" t="inlineStr"/>
-      <c r="D121" t="inlineStr"/>
+      <c r="C121" t="n">
+        <v>0</v>
+      </c>
+      <c r="D121" t="n">
+        <v>0</v>
+      </c>
       <c r="E121" t="n">
         <v>0</v>
       </c>
-      <c r="F121" t="inlineStr"/>
+      <c r="F121" t="n">
+        <v>0</v>
+      </c>
       <c r="G121" t="n">
         <v>0</v>
       </c>
@@ -5400,12 +5760,18 @@
       <c r="B124" t="n">
         <v>0</v>
       </c>
-      <c r="C124" t="inlineStr"/>
-      <c r="D124" t="inlineStr"/>
+      <c r="C124" t="n">
+        <v>0</v>
+      </c>
+      <c r="D124" t="n">
+        <v>0</v>
+      </c>
       <c r="E124" t="n">
         <v>0</v>
       </c>
-      <c r="F124" t="inlineStr"/>
+      <c r="F124" t="n">
+        <v>0</v>
+      </c>
       <c r="G124" t="n">
         <v>0</v>
       </c>
@@ -5436,12 +5802,18 @@
       <c r="B125" t="n">
         <v>0</v>
       </c>
-      <c r="C125" t="inlineStr"/>
-      <c r="D125" t="inlineStr"/>
+      <c r="C125" t="n">
+        <v>0</v>
+      </c>
+      <c r="D125" t="n">
+        <v>0</v>
+      </c>
       <c r="E125" t="n">
         <v>0</v>
       </c>
-      <c r="F125" t="inlineStr"/>
+      <c r="F125" t="n">
+        <v>0</v>
+      </c>
       <c r="G125" t="n">
         <v>0</v>
       </c>
@@ -5472,12 +5844,18 @@
       <c r="B126" t="n">
         <v>0</v>
       </c>
-      <c r="C126" t="inlineStr"/>
-      <c r="D126" t="inlineStr"/>
+      <c r="C126" t="n">
+        <v>0</v>
+      </c>
+      <c r="D126" t="n">
+        <v>0</v>
+      </c>
       <c r="E126" t="n">
         <v>0</v>
       </c>
-      <c r="F126" t="inlineStr"/>
+      <c r="F126" t="n">
+        <v>0</v>
+      </c>
       <c r="G126" t="n">
         <v>0</v>
       </c>
@@ -5816,12 +6194,18 @@
       <c r="B134" t="n">
         <v>0</v>
       </c>
-      <c r="C134" t="inlineStr"/>
-      <c r="D134" t="inlineStr"/>
+      <c r="C134" t="n">
+        <v>0</v>
+      </c>
+      <c r="D134" t="n">
+        <v>0</v>
+      </c>
       <c r="E134" t="n">
         <v>0</v>
       </c>
-      <c r="F134" t="inlineStr"/>
+      <c r="F134" t="n">
+        <v>0</v>
+      </c>
       <c r="G134" t="n">
         <v>0</v>
       </c>
@@ -6028,12 +6412,18 @@
       <c r="B139" t="n">
         <v>0</v>
       </c>
-      <c r="C139" t="inlineStr"/>
-      <c r="D139" t="inlineStr"/>
+      <c r="C139" t="n">
+        <v>0</v>
+      </c>
+      <c r="D139" t="n">
+        <v>0</v>
+      </c>
       <c r="E139" t="n">
         <v>0</v>
       </c>
-      <c r="F139" t="inlineStr"/>
+      <c r="F139" t="n">
+        <v>0</v>
+      </c>
       <c r="G139" t="n">
         <v>0</v>
       </c>
@@ -6284,12 +6674,18 @@
       <c r="B145" t="n">
         <v>0</v>
       </c>
-      <c r="C145" t="inlineStr"/>
-      <c r="D145" t="inlineStr"/>
+      <c r="C145" t="n">
+        <v>0</v>
+      </c>
+      <c r="D145" t="n">
+        <v>0</v>
+      </c>
       <c r="E145" t="n">
         <v>0</v>
       </c>
-      <c r="F145" t="inlineStr"/>
+      <c r="F145" t="n">
+        <v>0</v>
+      </c>
       <c r="G145" t="n">
         <v>0</v>
       </c>

</xml_diff>